<commit_message>
Ready to update to V2.
</commit_message>
<xml_diff>
--- a/GPIO.xlsx
+++ b/GPIO.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Onedrive\科研要紧\2021\IAS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Onedrive\科研要紧\2021\IAS\IntegratedAvionicsSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398CAB30-E7D1-48B6-8144-5C1FB8744A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20069B18-B98A-4AD3-BE6D-C6E1BCE50C74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{D7F7D35C-F34D-4D13-A132-7FAC7CDEDC53}"/>
   </bookViews>
   <sheets>
-    <sheet name="GPIO" sheetId="1" r:id="rId1"/>
-    <sheet name="SBLink" sheetId="2" r:id="rId2"/>
+    <sheet name="GPIO-New" sheetId="3" r:id="rId1"/>
+    <sheet name="GPIO" sheetId="1" r:id="rId2"/>
+    <sheet name="SBLink" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="177">
   <si>
     <t>GPIO</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -659,6 +660,22 @@
   </si>
   <si>
     <t>PWM_IN8</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADC</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPI_SCK</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPI_MISO</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPI_MOSI</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -807,7 +824,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -862,6 +879,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -882,6 +902,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1198,11 +1224,680 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD42C0F6-76A5-43A4-ACF4-5F0C1CB7F109}">
+  <dimension ref="A1:M36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.875" customWidth="1"/>
+    <col min="2" max="2" width="3.375" customWidth="1"/>
+    <col min="3" max="3" width="38.75" customWidth="1"/>
+    <col min="4" max="4" width="31" customWidth="1"/>
+    <col min="5" max="5" width="23.25" customWidth="1"/>
+    <col min="6" max="7" width="9.125" customWidth="1"/>
+    <col min="8" max="8" width="9.125" style="18" customWidth="1"/>
+    <col min="9" max="9" width="9.125" style="9" customWidth="1"/>
+    <col min="10" max="10" width="9.125" style="18" customWidth="1"/>
+    <col min="11" max="11" width="9.125" style="10" customWidth="1"/>
+    <col min="12" max="12" width="9.125" style="18" customWidth="1"/>
+    <col min="13" max="13" width="9" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1"/>
+      <c r="I1"/>
+      <c r="J1"/>
+      <c r="K1"/>
+      <c r="L1"/>
+      <c r="M1"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="H2" s="27"/>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="H3" s="27"/>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="H4" s="27"/>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="H5" s="27"/>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5" s="27"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="H6" s="27"/>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="H7" s="27"/>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="H8" s="27"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8" s="27"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="H9" s="27"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="27"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="H10" s="27"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="27"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="27"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13"/>
+      <c r="K13"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="27"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="27"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="H15" s="27"/>
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="H16" s="27"/>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16"/>
+      <c r="M16"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="H17" s="27"/>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="H18" s="27"/>
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
+      <c r="L18"/>
+      <c r="M18"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
+      <c r="M19"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20"/>
+      <c r="K20"/>
+      <c r="L20"/>
+      <c r="M20"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+      <c r="L21"/>
+      <c r="M21"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22"/>
+      <c r="L22"/>
+      <c r="M22"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" s="1"/>
+      <c r="E30" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA91FD8B-EC9E-4FAB-ABEB-3DEF11C8F37E}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1257,7 +1952,7 @@
       <c r="E2" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="19" t="s">
         <v>134</v>
       </c>
       <c r="I2" s="11" t="s">
@@ -1282,7 +1977,7 @@
       <c r="E3" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="H3" s="19"/>
+      <c r="H3" s="20"/>
       <c r="I3" s="11" t="s">
         <v>91</v>
       </c>
@@ -1290,10 +1985,10 @@
       <c r="K3" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="L3" s="22" t="s">
+      <c r="L3" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="22" t="s">
         <v>132</v>
       </c>
     </row>
@@ -1309,7 +2004,7 @@
       <c r="E4" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="H4" s="19"/>
+      <c r="H4" s="20"/>
       <c r="I4" s="11" t="s">
         <v>92</v>
       </c>
@@ -1317,8 +2012,8 @@
       <c r="K4" s="7">
         <v>3.3</v>
       </c>
-      <c r="L4" s="20"/>
-      <c r="M4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="22"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -1332,7 +2027,7 @@
       <c r="E5" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="H5" s="19"/>
+      <c r="H5" s="20"/>
       <c r="I5" s="11" t="s">
         <v>93</v>
       </c>
@@ -1343,7 +2038,7 @@
       <c r="L5" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="M5" s="21"/>
+      <c r="M5" s="22"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1354,7 +2049,7 @@
         <v>163</v>
       </c>
       <c r="D6" s="1"/>
-      <c r="H6" s="20"/>
+      <c r="H6" s="21"/>
       <c r="I6" s="11" t="s">
         <v>94</v>
       </c>
@@ -1362,10 +2057,10 @@
       <c r="K6" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="L6" s="18" t="s">
+      <c r="L6" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="M6" s="21"/>
+      <c r="M6" s="22"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1377,7 +2072,7 @@
       </c>
       <c r="D7" s="1"/>
       <c r="G7" s="16"/>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="19" t="s">
         <v>135</v>
       </c>
       <c r="I7" s="13" t="s">
@@ -1387,8 +2082,8 @@
       <c r="K7" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="L7" s="20"/>
-      <c r="M7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="22"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1400,7 +2095,7 @@
       </c>
       <c r="D8" s="1"/>
       <c r="G8" s="16"/>
-      <c r="H8" s="20"/>
+      <c r="H8" s="21"/>
       <c r="I8" s="13" t="s">
         <v>96</v>
       </c>
@@ -1411,7 +2106,7 @@
       <c r="L8" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="M8" s="21"/>
+      <c r="M8" s="22"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
@@ -1426,7 +2121,7 @@
         <v>168</v>
       </c>
       <c r="G9" s="17"/>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="19" t="s">
         <v>136</v>
       </c>
       <c r="I9" s="13" t="s">
@@ -1436,10 +2131,10 @@
       <c r="K9" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="L9" s="22" t="s">
+      <c r="L9" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="M9" s="21"/>
+      <c r="M9" s="22"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
@@ -1456,7 +2151,7 @@
         <v>144</v>
       </c>
       <c r="G10" s="16"/>
-      <c r="H10" s="20"/>
+      <c r="H10" s="21"/>
       <c r="I10" s="13" t="s">
         <v>98</v>
       </c>
@@ -1464,8 +2159,8 @@
       <c r="K10" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="L10" s="19"/>
-      <c r="M10" s="21"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="22"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
@@ -1489,8 +2184,8 @@
       <c r="K11" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="L11" s="19"/>
-      <c r="M11" s="21"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="22"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
@@ -1514,8 +2209,8 @@
       <c r="K12" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="L12" s="19"/>
-      <c r="M12" s="21"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="22"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
@@ -1539,8 +2234,8 @@
       <c r="K13" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="L13" s="20"/>
-      <c r="M13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="22"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
@@ -1562,10 +2257,10 @@
       <c r="K14" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="L14" s="21" t="s">
+      <c r="L14" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="M14" s="21" t="s">
+      <c r="M14" s="22" t="s">
         <v>131</v>
       </c>
     </row>
@@ -1581,7 +2276,7 @@
         <v>37</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="H15" s="22" t="s">
+      <c r="H15" s="23" t="s">
         <v>129</v>
       </c>
       <c r="I15" s="13" t="s">
@@ -1591,8 +2286,8 @@
       <c r="K15" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="L15" s="21"/>
-      <c r="M15" s="21"/>
+      <c r="L15" s="22"/>
+      <c r="M15" s="22"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
@@ -1606,7 +2301,7 @@
         <v>38</v>
       </c>
       <c r="E16" s="2"/>
-      <c r="H16" s="20"/>
+      <c r="H16" s="21"/>
       <c r="I16" s="13" t="s">
         <v>104</v>
       </c>
@@ -1630,7 +2325,7 @@
       </c>
       <c r="E17" s="2"/>
       <c r="G17" s="16"/>
-      <c r="H17" s="22" t="s">
+      <c r="H17" s="23" t="s">
         <v>130</v>
       </c>
       <c r="I17" s="13" t="s">
@@ -1652,7 +2347,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="4"/>
       <c r="G18" s="16"/>
-      <c r="H18" s="20"/>
+      <c r="H18" s="21"/>
       <c r="I18" s="13" t="s">
         <v>106</v>
       </c>
@@ -1985,7 +2680,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7E4174-8F8E-450E-8F71-1EA30FDB9AB0}">
   <dimension ref="A1:L23"/>
   <sheetViews>
@@ -2055,184 +2750,184 @@
       <c r="G2" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="I2" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="J2" s="23">
+      <c r="J2" s="24">
         <v>0</v>
       </c>
-      <c r="K2" s="23" t="s">
+      <c r="K2" s="24" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="I4" s="23" t="s">
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="I4" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="I6" s="23" t="s">
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="I6" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="I8" s="23" t="s">
+      <c r="I8" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="I10" s="23" t="s">
+      <c r="I10" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="I12" s="23" t="s">
+      <c r="I12" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="23"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="I14" s="23" t="s">
+      <c r="I14" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="I16" s="23" t="s">
+      <c r="I16" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
     </row>
     <row r="17" spans="9:11" x14ac:dyDescent="0.2">
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="23"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
     </row>
     <row r="18" spans="9:11" x14ac:dyDescent="0.2">
-      <c r="I18" s="23" t="s">
+      <c r="I18" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="J18" s="23"/>
-      <c r="K18" s="23"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
     </row>
     <row r="19" spans="9:11" x14ac:dyDescent="0.2">
-      <c r="I19" s="23"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="23"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
     </row>
     <row r="20" spans="9:11" x14ac:dyDescent="0.2">
-      <c r="I20" s="23" t="s">
+      <c r="I20" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="J20" s="23"/>
-      <c r="K20" s="23"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
     </row>
     <row r="21" spans="9:11" x14ac:dyDescent="0.2">
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="23"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
     </row>
     <row r="22" spans="9:11" x14ac:dyDescent="0.2">
-      <c r="I22" s="23" t="s">
+      <c r="I22" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="J22" s="23"/>
-      <c r="K22" s="23"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
     </row>
     <row r="23" spans="9:11" x14ac:dyDescent="0.2">
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="37">

</xml_diff>